<commit_message>
Add fxn to make ridge plot
</commit_message>
<xml_diff>
--- a/data-raw/Example questionnaire.xlsx
+++ b/data-raw/Example questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\opat\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AAF6637-D6AD-4487-B247-8157FDE612A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBCCA4D-1CDC-4BD5-9E1D-5AC1BA06D06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DCB68ECE-DBFD-4EA5-81CC-7203B783D8F9}"/>
   </bookViews>
@@ -958,7 +958,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,7 +1141,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -1152,7 +1152,7 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Add weight column to ex questionaire
</commit_message>
<xml_diff>
--- a/data-raw/Example questionnaire.xlsx
+++ b/data-raw/Example questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\opat\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBCCA4D-1CDC-4BD5-9E1D-5AC1BA06D06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EEB6E1-0BBD-4CFE-B4F0-F9911D945119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DCB68ECE-DBFD-4EA5-81CC-7203B783D8F9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>title</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>1.05</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>6.25</t>
   </si>
 </sst>
 </file>
@@ -955,40 +964,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23ED5A6-8E82-40C8-856E-7E2516780679}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C13" sqref="C13:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -996,19 +1005,22 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1016,74 +1028,92 @@
         <v>1</v>
       </c>
       <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1091,70 +1121,88 @@
         <v>1</v>
       </c>
       <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
         <v>5</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
         <v>4</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed example to be more bimodal
</commit_message>
<xml_diff>
--- a/data-raw/Example questionnaire.xlsx
+++ b/data-raw/Example questionnaire.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\opat\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\ADOPTpkg\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EEB6E1-0BBD-4CFE-B4F0-F9911D945119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E74D040-4EC7-44C3-B946-365F3EDEE849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DCB68ECE-DBFD-4EA5-81CC-7203B783D8F9}"/>
+    <workbookView xWindow="-34065" yWindow="6420" windowWidth="28800" windowHeight="15285" xr2:uid="{DCB68ECE-DBFD-4EA5-81CC-7203B783D8F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Example questionnaire" sheetId="1" r:id="rId1"/>
@@ -967,7 +967,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1124,7 @@
         <v>50</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1144,7 +1144,7 @@
         <v>26</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -1158,7 +1158,7 @@
         <v>27</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -1200,7 +1200,7 @@
         <v>26</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>

</xml_diff>